<commit_message>
bổ sung giống mèo burmese, bổ sung lại mô hình .keras , metadata
</commit_message>
<xml_diff>
--- a/ai/data/metadata.xlsx
+++ b/ai/data/metadata.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="660">
   <si>
     <t>STT</t>
   </si>
@@ -2762,6 +2762,21 @@
   </si>
   <si>
     <t>score_size</t>
+  </si>
+  <si>
+    <t>burmese</t>
+  </si>
+  <si>
+    <t>40 – 46 cm</t>
+  </si>
+  <si>
+    <t>800 – 2000 USD</t>
+  </si>
+  <si>
+    <t>type tên giống loài tuổi thọ trung bình cân nặng trung bình chiều cao trung bình chiều dài trung bình cách chăm giá có giấy tờ giá không giấy tờ giá quốc tế
+Cat burmese 12 năm – 16 năm 3 – 6 kg 25 – 30 cm 40 – 46 cm "Burmese là giống mèo thân thiện, thông minh và rất quấn người, vì vậy chúng cần được quan tâm và tương tác thường xuyên. Về chế độ ăn, Burmese có cơ địa săn chắc, nhiều cơ bắp nên cần thức ăn giàu đạm động vật, ưu tiên các loại thức ăn chất lượng cao dành cho mèo trưởng thành. Có thể kết hợp thức ăn hạt và pate ướt để đảm bảo đủ dinh dưỡng và hạn chế các vấn đề về thận.
+Về vận động, Burmese khá hiếu động và thích chơi đùa, leo trèo. Chủ nuôi nên chuẩn bị đồ chơi, trụ cào móng hoặc không gian leo trèo trong nhà để giúp mèo giải tỏa năng lượng và tránh buồn chán. Chúng thích ở trong nhà và không cần ra ngoài thường xuyên như một số giống mèo khác.
+Về sức khỏe, Burmese nhìn chung khỏe mạnh nhưng có thể gặp một số vấn đề di truyền như bệnh nướu răng hoặc bệnh tim nhẹ. Việc vệ sinh răng miệng định kỳ, khám thú y thường xuyên và tiêm phòng đầy đủ là rất quan trọng. Tính cách của Burmese rất tình cảm, hòa đồng với trẻ em và các vật nuôi khác, phù hợp với gia đình cần một giống mèo thân thiện, gắn bó và dễ chăm sóc.</t>
   </si>
 </sst>
 </file>
@@ -2806,13 +2821,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3147,10 +3162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P140"/>
+  <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
@@ -3225,13 +3240,13 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>434</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -3260,13 +3275,13 @@
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>437</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -3295,13 +3310,13 @@
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>440</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -3330,13 +3345,13 @@
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>442</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -3365,13 +3380,13 @@
       <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>445</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -3400,13 +3415,13 @@
       <c r="D7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>448</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -3435,13 +3450,13 @@
       <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>437</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -3470,13 +3485,13 @@
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>451</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -3505,13 +3520,13 @@
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>454</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -3540,13 +3555,13 @@
       <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>454</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -3575,13 +3590,13 @@
       <c r="D12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>459</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -3610,13 +3625,13 @@
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>461</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -3645,13 +3660,13 @@
       <c r="D14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>464</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -3680,13 +3695,13 @@
       <c r="D15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>467</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -3715,13 +3730,13 @@
       <c r="D16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -3750,13 +3765,13 @@
       <c r="D17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>467</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -3785,13 +3800,13 @@
       <c r="D18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -3820,13 +3835,13 @@
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>467</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -3855,13 +3870,13 @@
       <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="1" t="s">
         <v>477</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -3890,13 +3905,13 @@
       <c r="D21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>480</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -3925,13 +3940,13 @@
       <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -3960,13 +3975,13 @@
       <c r="D23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -3995,13 +4010,13 @@
       <c r="D24" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -4030,13 +4045,13 @@
       <c r="D25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>491</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -4065,13 +4080,13 @@
       <c r="D26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>464</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -4100,13 +4115,13 @@
       <c r="D27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -4135,13 +4150,13 @@
       <c r="D28" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
         <v>496</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -4170,13 +4185,13 @@
       <c r="D29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -4205,13 +4220,13 @@
       <c r="D30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -4240,13 +4255,13 @@
       <c r="D31" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -4275,13 +4290,13 @@
       <c r="D32" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -4310,13 +4325,13 @@
       <c r="D33" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -4345,13 +4360,13 @@
       <c r="D34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -4380,13 +4395,13 @@
       <c r="D35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="1" t="s">
         <v>511</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -4415,13 +4430,13 @@
       <c r="D36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -4450,13 +4465,13 @@
       <c r="D37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -4485,13 +4500,13 @@
       <c r="D38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="1" t="s">
         <v>518</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -4523,10 +4538,10 @@
       <c r="E39" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="1" t="s">
         <v>521</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -4555,13 +4570,13 @@
       <c r="D40" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>521</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -4590,13 +4605,13 @@
       <c r="D41" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -4625,13 +4640,13 @@
       <c r="D42" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -4660,13 +4675,13 @@
       <c r="D43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="1" t="s">
         <v>530</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -4695,13 +4710,13 @@
       <c r="D44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="1" t="s">
         <v>533</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -4730,13 +4745,13 @@
       <c r="D45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="1" t="s">
         <v>534</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -4765,13 +4780,13 @@
       <c r="D46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -4800,13 +4815,13 @@
       <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="1" t="s">
         <v>539</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -4835,13 +4850,13 @@
       <c r="D48" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -4870,13 +4885,13 @@
       <c r="D49" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -4905,10 +4920,10 @@
       <c r="D50" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="1" t="s">
         <v>544</v>
       </c>
       <c r="G50" s="1" t="s">
@@ -4940,13 +4955,13 @@
       <c r="D51" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -4975,13 +4990,13 @@
       <c r="D52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -5010,13 +5025,13 @@
       <c r="D53" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -5045,13 +5060,13 @@
       <c r="D54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="1" t="s">
         <v>533</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -5080,13 +5095,13 @@
       <c r="D55" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="1" t="s">
         <v>533</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -5115,13 +5130,13 @@
       <c r="D56" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -5150,13 +5165,13 @@
       <c r="D57" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -5185,13 +5200,13 @@
       <c r="D58" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -5220,13 +5235,13 @@
       <c r="D59" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -5255,13 +5270,13 @@
       <c r="D60" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -5290,13 +5305,13 @@
       <c r="D61" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -5325,13 +5340,13 @@
       <c r="D62" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>557</v>
       </c>
       <c r="H62" s="1" t="s">
@@ -5360,13 +5375,13 @@
       <c r="D63" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H63" s="1" t="s">
@@ -5395,13 +5410,13 @@
       <c r="D64" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -5430,13 +5445,13 @@
       <c r="D65" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -5465,13 +5480,13 @@
       <c r="D66" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="1" t="s">
         <v>541</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -5500,13 +5515,13 @@
       <c r="D67" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H67" s="1" t="s">
@@ -5535,13 +5550,13 @@
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="1" t="s">
         <v>491</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -5570,13 +5585,13 @@
       <c r="D69" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="1" t="s">
         <v>541</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -5605,13 +5620,13 @@
       <c r="D70" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="1" t="s">
         <v>511</v>
       </c>
       <c r="H70" s="1" t="s">
@@ -5640,13 +5655,13 @@
       <c r="D71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H71" s="1" t="s">
@@ -5675,13 +5690,13 @@
       <c r="D72" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H72" s="1" t="s">
@@ -5710,13 +5725,13 @@
       <c r="D73" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H73" s="1" t="s">
@@ -5745,13 +5760,13 @@
       <c r="D74" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" s="1" t="s">
         <v>530</v>
       </c>
       <c r="H74" s="1" t="s">
@@ -5780,13 +5795,13 @@
       <c r="D75" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H75" s="1" t="s">
@@ -5815,13 +5830,13 @@
       <c r="D76" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H76" s="1" t="s">
@@ -5850,13 +5865,13 @@
       <c r="D77" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="2" t="s">
         <v>499</v>
       </c>
       <c r="H77" s="1" t="s">
@@ -5885,13 +5900,13 @@
       <c r="D78" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G78" s="2" t="s">
         <v>541</v>
       </c>
       <c r="H78" s="1" t="s">
@@ -5920,10 +5935,10 @@
       <c r="D79" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="1" t="s">
         <v>485</v>
       </c>
       <c r="G79" s="1" t="s">
@@ -5955,13 +5970,13 @@
       <c r="D80" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H80" s="1" t="s">
@@ -5990,13 +6005,13 @@
       <c r="D81" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H81" s="1" t="s">
@@ -6025,13 +6040,13 @@
       <c r="D82" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="1" t="s">
         <v>488</v>
       </c>
       <c r="H82" s="1" t="s">
@@ -6060,13 +6075,13 @@
       <c r="D83" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="1" t="s">
         <v>491</v>
       </c>
       <c r="H83" s="1" t="s">
@@ -6095,13 +6110,13 @@
       <c r="D84" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H84" s="1" t="s">
@@ -6130,13 +6145,13 @@
       <c r="D85" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H85" s="1" t="s">
@@ -6165,10 +6180,10 @@
       <c r="D86" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="1" t="s">
         <v>504</v>
       </c>
       <c r="G86" s="1" t="s">
@@ -6200,13 +6215,13 @@
       <c r="D87" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="1" t="s">
         <v>499</v>
       </c>
       <c r="H87" s="1" t="s">
@@ -6235,13 +6250,13 @@
       <c r="D88" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H88" s="1" t="s">
@@ -6270,13 +6285,13 @@
       <c r="D89" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="1" t="s">
         <v>464</v>
       </c>
       <c r="H89" s="1" t="s">
@@ -6305,13 +6320,13 @@
       <c r="D90" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H90" s="1" t="s">
@@ -6340,13 +6355,13 @@
       <c r="D91" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H91" s="1" t="s">
@@ -6375,13 +6390,13 @@
       <c r="D92" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H92" s="1" t="s">
@@ -6410,13 +6425,13 @@
       <c r="D93" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H93" s="1" t="s">
@@ -6445,13 +6460,13 @@
       <c r="D94" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="1" t="s">
         <v>469</v>
       </c>
       <c r="H94" s="1" t="s">
@@ -6480,13 +6495,13 @@
       <c r="D95" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="1" t="s">
         <v>464</v>
       </c>
       <c r="H95" s="1" t="s">
@@ -6515,13 +6530,13 @@
       <c r="D96" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="1" t="s">
         <v>605</v>
       </c>
       <c r="H96" s="1" t="s">
@@ -6550,13 +6565,13 @@
       <c r="D97" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="1" t="s">
         <v>606</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="1" t="s">
         <v>496</v>
       </c>
       <c r="H97" s="1" t="s">
@@ -6585,13 +6600,13 @@
       <c r="D98" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="1" t="s">
         <v>610</v>
       </c>
       <c r="H98" s="1" t="s">
@@ -6620,13 +6635,13 @@
       <c r="D99" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="1" t="s">
         <v>511</v>
       </c>
       <c r="H99" s="1" t="s">
@@ -6655,10 +6670,10 @@
       <c r="D100" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="1" t="s">
         <v>473</v>
       </c>
       <c r="G100" s="1" t="s">
@@ -6690,13 +6705,13 @@
       <c r="D101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G101" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H101" s="1" t="s">
@@ -6725,13 +6740,13 @@
       <c r="D102" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H102" s="1" t="s">
@@ -6760,13 +6775,13 @@
       <c r="D103" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G103" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H103" s="1" t="s">
@@ -6795,13 +6810,13 @@
       <c r="D104" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G104" s="1" t="s">
         <v>514</v>
       </c>
       <c r="H104" s="1" t="s">
@@ -6830,13 +6845,13 @@
       <c r="D105" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F105" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G105" s="1" t="s">
         <v>496</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -6865,13 +6880,13 @@
       <c r="D106" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G106" s="1" t="s">
         <v>496</v>
       </c>
       <c r="H106" s="1" t="s">
@@ -6900,13 +6915,13 @@
       <c r="D107" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="1" t="s">
         <v>496</v>
       </c>
       <c r="H107" s="1" t="s">
@@ -6935,13 +6950,13 @@
       <c r="D108" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="F108" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G108" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H108" s="1" t="s">
@@ -6970,13 +6985,13 @@
       <c r="D109" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F109" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G109" s="1" t="s">
         <v>439</v>
       </c>
       <c r="H109" s="1" t="s">
@@ -7005,13 +7020,13 @@
       <c r="D110" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H110" s="1" t="s">
@@ -7040,13 +7055,13 @@
       <c r="D111" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" s="1" t="s">
         <v>541</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -7075,13 +7090,13 @@
       <c r="D112" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112" s="1" t="s">
         <v>439</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -7113,10 +7128,10 @@
       <c r="E113" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" s="1" t="s">
         <v>504</v>
       </c>
       <c r="H113" s="1" t="s">
@@ -7145,13 +7160,13 @@
       <c r="D114" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" s="1" t="s">
         <v>541</v>
       </c>
       <c r="H114" s="1" t="s">
@@ -7180,13 +7195,13 @@
       <c r="D115" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G115" s="1" t="s">
         <v>634</v>
       </c>
       <c r="H115" s="1" t="s">
@@ -7215,13 +7230,13 @@
       <c r="D116" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116" s="1" t="s">
         <v>539</v>
       </c>
       <c r="H116" s="1" t="s">
@@ -7250,13 +7265,13 @@
       <c r="D117" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F117" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117" s="1" t="s">
         <v>527</v>
       </c>
       <c r="H117" s="1" t="s">
@@ -7285,13 +7300,13 @@
       <c r="D118" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F118" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G118" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H118" s="1" t="s">
@@ -7320,13 +7335,13 @@
       <c r="D119" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G119" s="1" t="s">
         <v>557</v>
       </c>
       <c r="H119" s="1" t="s">
@@ -7355,13 +7370,13 @@
       <c r="D120" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120" s="1" t="s">
         <v>641</v>
       </c>
       <c r="H120" s="1" t="s">
@@ -7390,13 +7405,13 @@
       <c r="D121" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G121" s="1" t="s">
         <v>644</v>
       </c>
       <c r="H121" s="1" t="s">
@@ -7425,13 +7440,13 @@
       <c r="D122" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F122" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" s="1" t="s">
         <v>534</v>
       </c>
       <c r="H122" s="1" t="s">
@@ -7460,13 +7475,13 @@
       <c r="D123" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="F123" t="s">
+      <c r="F123" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H123" s="1" t="s">
@@ -7495,13 +7510,13 @@
       <c r="D124" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G124" t="s">
+      <c r="G124" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H124" s="1" t="s">
@@ -7530,13 +7545,13 @@
       <c r="D125" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="F125" t="s">
+      <c r="F125" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125" s="1" t="s">
         <v>534</v>
       </c>
       <c r="H125" s="1" t="s">
@@ -7565,13 +7580,13 @@
       <c r="D126" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="F126" t="s">
+      <c r="F126" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H126" s="1" t="s">
@@ -7600,13 +7615,13 @@
       <c r="D127" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F127" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" s="1" t="s">
         <v>609</v>
       </c>
       <c r="H127" s="1" t="s">
@@ -7635,13 +7650,13 @@
       <c r="D128" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F128" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G128" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H128" s="1" t="s">
@@ -7670,13 +7685,13 @@
       <c r="D129" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G129" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H129" s="1" t="s">
@@ -7705,13 +7720,13 @@
       <c r="D130" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F130" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="G130" s="4" t="s">
+      <c r="G130" s="3" t="s">
         <v>649</v>
       </c>
       <c r="H130" s="1" t="s">
@@ -7740,13 +7755,13 @@
       <c r="D131" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G131" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H131" s="1" t="s">
@@ -7775,13 +7790,13 @@
       <c r="D132" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="F132" t="s">
+      <c r="F132" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G132" t="s">
+      <c r="G132" s="1" t="s">
         <v>534</v>
       </c>
       <c r="H132" s="1" t="s">
@@ -7810,13 +7825,13 @@
       <c r="D133" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G133" s="1" t="s">
         <v>511</v>
       </c>
       <c r="H133" s="1" t="s">
@@ -7845,13 +7860,13 @@
       <c r="D134" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="F134" t="s">
+      <c r="F134" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G134" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H134" s="1" t="s">
@@ -7880,13 +7895,13 @@
       <c r="D135" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F135" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G135" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H135" s="1" t="s">
@@ -7915,13 +7930,13 @@
       <c r="D136" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F136" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G136" t="s">
+      <c r="G136" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H136" s="1" t="s">
@@ -7950,13 +7965,13 @@
       <c r="D137" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="F137" t="s">
+      <c r="F137" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G137" t="s">
+      <c r="G137" s="1" t="s">
         <v>534</v>
       </c>
       <c r="H137" s="1" t="s">
@@ -7985,13 +8000,13 @@
       <c r="D138" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="F138" t="s">
+      <c r="F138" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="G138" t="s">
+      <c r="G138" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H138" s="1" t="s">
@@ -8020,13 +8035,13 @@
       <c r="D139" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="F139" t="s">
+      <c r="F139" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G139" t="s">
+      <c r="G139" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H139" s="1" t="s">
@@ -8055,13 +8070,13 @@
       <c r="D140" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="F140" t="s">
+      <c r="F140" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="1" t="s">
         <v>482</v>
       </c>
       <c r="H140" s="1" t="s">
@@ -8075,6 +8090,41 @@
       </c>
       <c r="K140" s="1" t="s">
         <v>428</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>